<commit_message>
trying to use latest data
For more accurate modeling. Saving before using the LoadMatFile_SaveAsCSV.m file in case it saves things incorrectly.
</commit_message>
<xml_diff>
--- a/BPA_Static_Characterization_Test/DataCollection/BPAparameters_.xlsx
+++ b/BPA_Static_Characterization_Test/DataCollection/BPAparameters_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory_2\Muscle_Sensory\DataCollection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Muscle_Sensory\BPA_Static_Characterization_Test\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AD6CE6B-BF2F-40A7-8E80-5C894FAF213F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A6BB67-76D0-4128-9B37-099F9980B91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
   </bookViews>
   <sheets>
     <sheet name="10mm" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -410,32 +413,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -448,40 +445,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -490,10 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -520,22 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -544,10 +511,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2983,15 +2950,15 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3017,7 +2984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>13.5</v>
       </c>
@@ -3030,14 +2997,14 @@
       <c r="D2" s="3">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F2">
         <f>A2-B2</f>
         <v>1.5</v>
       </c>
-      <c r="I2" s="31">
+      <c r="I2" s="25">
         <v>13.5</v>
       </c>
       <c r="J2" s="2">
@@ -3046,18 +3013,16 @@
       <c r="K2" s="2">
         <v>10</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="19">
         <v>12</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>11.6</v>
       </c>
       <c r="F3">
@@ -3065,17 +3030,13 @@
         <v>0</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="26">
+      <c r="L3" s="20">
         <v>11.6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>11.2</v>
       </c>
       <c r="F4">
@@ -3087,31 +3048,29 @@
         <v>0</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="26">
+      <c r="L4" s="20">
         <v>11.2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8">
         <v>10.8</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="27">
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="21">
         <v>10.8</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>23</v>
       </c>
@@ -3121,17 +3080,17 @@
       <c r="C6" s="2">
         <v>18.600000000000001</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="3">
         <v>21.9</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>1.1000000000000014</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="26">
         <v>23.6</v>
       </c>
       <c r="J6" s="2">
@@ -3140,18 +3099,16 @@
       <c r="K6" s="2">
         <v>18.600000000000001</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="19">
         <v>21.9</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="12">
+      <c r="D7" s="5">
         <v>20.5</v>
       </c>
       <c r="F7">
@@ -3159,31 +3116,29 @@
         <v>0</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="26">
+      <c r="L7" s="20">
         <v>20.5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="13">
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8">
         <v>18.899999999999999</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="27">
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="21">
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>27.6</v>
       </c>
@@ -3193,17 +3148,17 @@
       <c r="C9" s="2">
         <v>22.1</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="3">
         <v>25.7</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>1.9000000000000021</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="25">
         <v>27.6</v>
       </c>
       <c r="J9" s="2">
@@ -3212,74 +3167,66 @@
       <c r="K9" s="2">
         <v>22.1</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="19">
         <v>25.7</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="M9" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="12">
+      <c r="D10" s="5">
         <v>25</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="9"/>
       <c r="F10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="26">
+      <c r="L10" s="20">
         <v>25</v>
       </c>
-      <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="12">
+      <c r="D11" s="5">
         <v>24.2</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="9"/>
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="26">
+      <c r="L11" s="20">
         <v>24.2</v>
       </c>
-      <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="13">
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8">
         <v>22.6</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="9"/>
       <c r="F12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="27">
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="21">
         <v>22.6</v>
       </c>
-      <c r="M12" s="10"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>29.8</v>
       </c>
@@ -3289,17 +3236,17 @@
       <c r="C13" s="2">
         <v>23.6</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="3">
         <v>28.1</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
         <v>1.6999999999999993</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="25">
         <v>29.8</v>
       </c>
       <c r="J13" s="2">
@@ -3308,162 +3255,154 @@
       <c r="K13" s="2">
         <v>23.6</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="19">
         <v>28.1</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="M13" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="12">
+      <c r="D14" s="5">
         <v>26.4</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="9"/>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="26">
+      <c r="L14" s="20">
         <v>26.4</v>
       </c>
-      <c r="M14" s="10"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="12">
+      <c r="D15" s="5">
         <v>25.3</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="9"/>
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="26">
+      <c r="L15" s="20">
         <v>25.3</v>
       </c>
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="13">
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8">
         <v>24</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="9"/>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="27">
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="21">
         <v>24</v>
       </c>
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
         <v>30</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="12">
         <v>28.1</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="12">
         <v>24</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="13">
         <v>28.1</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>1.8999999999999986</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="11">
         <v>30</v>
       </c>
-      <c r="J17" s="16">
+      <c r="J17" s="12">
         <v>28.1</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="12">
         <v>24</v>
       </c>
-      <c r="L17" s="28">
+      <c r="L17" s="22">
         <v>28.1</v>
       </c>
-      <c r="M17" s="10" t="s">
+      <c r="M17" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="14">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="10">
         <v>26.9</v>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="9"/>
       <c r="F18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="29">
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="23">
         <v>26.9</v>
       </c>
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="14">
+      <c r="M18" s="9"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="10">
         <v>25.9</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="29">
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="23">
         <v>25.9</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22">
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18">
         <v>24.8</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="30">
+      <c r="I20" s="16"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="24">
         <v>24.8</v>
       </c>
     </row>
@@ -3481,14 +3420,14 @@
       <selection sqref="A1:G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3502,20 +3441,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="26">
         <v>13.7</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="27">
         <v>12</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="27">
         <v>10</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="19">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G2">
@@ -3523,11 +3462,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="26">
+      <c r="D3" s="20">
         <v>11.6</v>
       </c>
       <c r="G3">
@@ -3535,11 +3472,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="26">
+      <c r="D4" s="20">
         <v>11.2</v>
       </c>
       <c r="G4">
@@ -3547,11 +3482,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="27">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="21">
         <v>10.8</v>
       </c>
       <c r="G5">
@@ -3559,20 +3494,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="26">
         <v>23.7</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="27">
         <v>22</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="27">
         <v>18.5</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="19">
         <v>21.9</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G6">
@@ -3580,11 +3515,9 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="26">
+      <c r="D7" s="20">
         <v>20.5</v>
       </c>
       <c r="G7">
@@ -3592,11 +3525,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="27">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="21">
         <v>18.899999999999999</v>
       </c>
       <c r="G8">
@@ -3604,20 +3537,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="26">
         <v>27.7</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="27">
         <v>26</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="27">
         <v>21.8</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="19">
         <v>25.7</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G9">
@@ -3625,59 +3558,55 @@
         <v>4.1999999999999993</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="26">
+      <c r="D10" s="20">
         <v>25</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="9"/>
       <c r="G10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="26">
+      <c r="D11" s="20">
         <v>24.2</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="9"/>
       <c r="G11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="27">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="21">
         <v>22.6</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="9"/>
       <c r="G12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="32">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="26">
         <v>29.7</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="27">
         <v>28.1</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="27">
         <v>23.5</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="19">
         <v>28.1</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="G13">
@@ -3685,59 +3614,55 @@
         <v>4.6000000000000014</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="26">
+      <c r="D14" s="20">
         <v>26.4</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="9"/>
       <c r="G14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="26">
+      <c r="D15" s="20">
         <v>25.3</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="9"/>
       <c r="G15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="27">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="21">
         <v>24</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="9"/>
       <c r="G16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
         <v>30</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="12">
         <v>28.1</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="12">
         <v>24</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="22">
         <v>28.1</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G17">
@@ -3745,28 +3670,28 @@
         <v>4.1000000000000014</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="29">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="23">
         <v>26.9</v>
       </c>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="29">
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="23">
         <v>25.9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="30">
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="24">
         <v>24.8</v>
       </c>
     </row>
@@ -3779,1136 +3704,1122 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6CD35F-74A9-469A-95AE-E3CD27253D58}">
   <dimension ref="B1:M48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="34"/>
-    <col min="2" max="2" width="16.85546875" style="34" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="34" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="34"/>
+    <col min="1" max="1" width="9.109375" style="28"/>
+    <col min="2" max="2" width="16.88671875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="28" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="28" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="29">
         <v>10</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="30">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="30">
         <v>7</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="30">
         <f t="shared" ref="E2:E7" si="0">(C2-D2)/C2</f>
         <v>0.15662650602409645</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="30">
         <f>C2-D2</f>
         <v>1.3000000000000007</v>
       </c>
-      <c r="G2" s="37">
+      <c r="G2" s="30">
         <f>B2-C2</f>
         <v>1.6999999999999993</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="40">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="33">
         <v>15</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="28">
         <v>13.2</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="28">
         <v>11.1</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="28">
         <f t="shared" si="0"/>
         <v>0.15909090909090906</v>
       </c>
-      <c r="F3" s="41">
+      <c r="F3" s="28">
         <f t="shared" ref="F3:F7" si="1">C3-D3</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="G3" s="42">
+      <c r="G3" s="28">
         <f t="shared" ref="G3:G7" si="2">B3-C3</f>
         <v>1.8000000000000007</v>
       </c>
-      <c r="H3" s="41">
+      <c r="H3" s="28">
         <v>639</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="40">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="33">
         <v>20</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="28">
         <v>18.2</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="28">
         <v>15.2</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="28">
         <f t="shared" si="0"/>
         <v>0.16483516483516483</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4" s="28">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G4" s="42">
+      <c r="G4" s="28">
         <f t="shared" si="2"/>
         <v>1.8000000000000007</v>
       </c>
-      <c r="H4" s="41">
+      <c r="H4" s="28">
         <v>640</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="40">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="33">
         <v>25</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="28">
         <v>23.3</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="28">
         <v>19.3</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="28">
         <f t="shared" si="0"/>
         <v>0.17167381974248927</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5" s="28">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G5" s="42">
+      <c r="G5" s="28">
         <f t="shared" si="2"/>
         <v>1.6999999999999993</v>
       </c>
-      <c r="H5" s="41">
+      <c r="H5" s="28">
         <v>640</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="44">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="35">
         <v>30</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="36">
         <v>28.1</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="36">
         <v>23.2</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="36">
         <f t="shared" si="0"/>
         <v>0.17437722419928833</v>
       </c>
-      <c r="F6" s="41">
+      <c r="F6" s="28">
         <f t="shared" si="1"/>
         <v>4.9000000000000021</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="28">
         <f t="shared" si="2"/>
         <v>1.8999999999999986</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H6" s="28">
         <v>639</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="46">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="33">
         <v>40</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="28">
         <v>38.200000000000003</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="28">
         <v>31.4</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="28">
         <f t="shared" si="0"/>
         <v>0.17801047120418859</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F7" s="28">
         <f t="shared" si="1"/>
         <v>6.8000000000000043</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G7" s="28">
         <f t="shared" si="2"/>
         <v>1.7999999999999972</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="28">
         <v>640</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="50"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
+    <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="37"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="39"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="34" t="s">
+    <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="34" t="s">
+      <c r="G16" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="35">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="29">
         <v>10</v>
       </c>
-      <c r="C17" s="36">
+      <c r="C17" s="30">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="30">
         <v>7</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="30">
         <f t="shared" ref="E17:E23" si="3">(C17-D17)/C17</f>
         <v>0.15662650602409645</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37">
+      <c r="F17" s="30"/>
+      <c r="G17" s="30">
         <f>B17-C17</f>
         <v>1.6999999999999993</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="31">
         <v>620</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="40">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="33">
         <v>15</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="28">
         <v>13.2</v>
       </c>
-      <c r="D18" s="41">
+      <c r="D18" s="28">
         <v>11.1</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="28">
         <f t="shared" si="3"/>
         <v>0.15909090909090906</v>
       </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="42">
+      <c r="G18" s="28">
         <f t="shared" ref="G18:G23" si="4">B18-C18</f>
         <v>1.8000000000000007</v>
       </c>
-      <c r="H18" s="41">
+      <c r="H18" s="28">
         <v>630</v>
       </c>
-      <c r="I18" s="43"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="40">
+      <c r="I18" s="34"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="33">
         <v>20</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41" t="e">
+      <c r="E19" s="28" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F19" s="41"/>
-      <c r="G19" s="42">
+      <c r="G19" s="28">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="H19" s="41"/>
-      <c r="I19" s="43"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="40">
+      <c r="I19" s="34"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="33">
         <v>25</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41" t="e">
+      <c r="E20" s="28" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42">
+      <c r="G20" s="28">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="H20" s="41"/>
-      <c r="I20" s="43"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="44">
+      <c r="I20" s="34"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="35">
         <v>30</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45" t="e">
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F21" s="45"/>
-      <c r="G21" s="42">
+      <c r="F21" s="36"/>
+      <c r="G21" s="28">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="H21" s="41"/>
-      <c r="I21" s="43"/>
-    </row>
-    <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="46">
+      <c r="I21" s="34"/>
+    </row>
+    <row r="22" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="33">
         <v>40</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42" t="e">
+      <c r="E22" s="28" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42">
+      <c r="G22" s="28">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="H22" s="42"/>
-      <c r="I22" s="43"/>
-    </row>
-    <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="51">
+      <c r="I22" s="34"/>
+    </row>
+    <row r="23" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="40">
         <v>44.5</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52" t="e">
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F23" s="52"/>
-      <c r="G23" s="53">
+      <c r="F23" s="41"/>
+      <c r="G23" s="42">
         <f t="shared" si="4"/>
         <v>44.5</v>
       </c>
-      <c r="H23" s="48"/>
-      <c r="I23" s="50"/>
-    </row>
-    <row r="25" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G25" s="34" t="s">
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
+    </row>
+    <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G26" s="54">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G26" s="43">
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G27" s="55">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G27" s="44">
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="34" t="s">
+    <row r="28" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="55">
+      <c r="G28" s="44">
         <v>0.75</v>
       </c>
-      <c r="J28" s="34" t="s">
+      <c r="J28" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="56" t="s">
+    <row r="29" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="57" t="s">
+      <c r="D29" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="E29" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="57" t="s">
+      <c r="F29" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="57" t="s">
+      <c r="G29" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="57" t="s">
+      <c r="H29" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I29" s="57" t="s">
+      <c r="I29" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="J29" s="57" t="s">
+      <c r="J29" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="K29" s="57" t="s">
+      <c r="K29" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="L29" s="57" t="s">
+      <c r="L29" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="M29" s="58" t="s">
+      <c r="M29" s="47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="46">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="33">
         <v>10</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="28">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D30" s="41">
+      <c r="D30" s="28">
         <v>7</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="28">
         <f t="shared" ref="E30:E36" si="5">(C30-D30)/C30</f>
         <v>0.15662650602409645</v>
       </c>
-      <c r="F30" s="41">
+      <c r="F30" s="28">
         <f>C30-D30</f>
         <v>1.3000000000000007</v>
       </c>
-      <c r="G30" s="59">
+      <c r="G30" s="29">
         <f t="shared" ref="G30:G36" si="6">$G$26*F30</f>
         <v>0.32500000000000018</v>
       </c>
-      <c r="H30" s="54">
+      <c r="H30" s="43">
         <f t="shared" ref="H30:H36" si="7">$G$27*F30</f>
         <v>0.65000000000000036</v>
       </c>
-      <c r="I30" s="60">
+      <c r="I30" s="32">
         <f t="shared" ref="I30:I36" si="8">$G$28*F30</f>
         <v>0.97500000000000053</v>
       </c>
-      <c r="J30" s="37">
+      <c r="J30" s="30">
         <f>C30</f>
         <v>8.3000000000000007</v>
       </c>
-      <c r="K30" s="37">
+      <c r="K30" s="30">
         <f>C30-G30</f>
         <v>7.9750000000000005</v>
       </c>
-      <c r="L30" s="37">
+      <c r="L30" s="30">
         <f>C30-H30</f>
         <v>7.65</v>
       </c>
-      <c r="M30" s="60">
+      <c r="M30" s="32">
         <f>C30-I30</f>
         <v>7.3250000000000002</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="46">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="33">
         <v>15</v>
       </c>
-      <c r="C31" s="41">
+      <c r="C31" s="28">
         <v>13.2</v>
       </c>
-      <c r="D31" s="41">
+      <c r="D31" s="28">
         <v>11.1</v>
       </c>
-      <c r="E31" s="41">
+      <c r="E31" s="28">
         <f t="shared" si="5"/>
         <v>0.15909090909090906</v>
       </c>
-      <c r="F31" s="41">
+      <c r="F31" s="28">
         <f t="shared" ref="F31:F36" si="9">C31-D31</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="G31" s="46">
+      <c r="G31" s="33">
         <f t="shared" si="6"/>
         <v>0.52499999999999991</v>
       </c>
-      <c r="H31" s="55">
+      <c r="H31" s="44">
         <f t="shared" si="7"/>
         <v>1.0499999999999998</v>
       </c>
-      <c r="I31" s="61">
+      <c r="I31" s="34">
         <f t="shared" si="8"/>
         <v>1.5749999999999997</v>
       </c>
-      <c r="J31" s="42">
+      <c r="J31" s="28">
         <f t="shared" ref="J31:J36" si="10">C31</f>
         <v>13.2</v>
       </c>
-      <c r="K31" s="42">
+      <c r="K31" s="28">
         <f t="shared" ref="K31:K36" si="11">C31-G31</f>
         <v>12.674999999999999</v>
       </c>
-      <c r="L31" s="42">
+      <c r="L31" s="28">
         <f t="shared" ref="L31:L36" si="12">C31-H31</f>
         <v>12.149999999999999</v>
       </c>
-      <c r="M31" s="61">
+      <c r="M31" s="34">
         <f t="shared" ref="M31:M36" si="13">C31-I31</f>
         <v>11.625</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="46">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="33">
         <v>20</v>
       </c>
-      <c r="C32" s="41">
+      <c r="C32" s="28">
         <v>18.2</v>
       </c>
-      <c r="D32" s="41">
+      <c r="D32" s="28">
         <v>15.2</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="28">
         <f t="shared" si="5"/>
         <v>0.16483516483516483</v>
       </c>
-      <c r="F32" s="41">
+      <c r="F32" s="28">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="G32" s="46">
+      <c r="G32" s="33">
         <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
-      <c r="H32" s="55">
+      <c r="H32" s="44">
         <f t="shared" si="7"/>
         <v>1.5</v>
       </c>
-      <c r="I32" s="61">
+      <c r="I32" s="34">
         <f t="shared" si="8"/>
         <v>2.25</v>
       </c>
-      <c r="J32" s="42">
+      <c r="J32" s="28">
         <f t="shared" si="10"/>
         <v>18.2</v>
       </c>
-      <c r="K32" s="42">
+      <c r="K32" s="28">
         <f t="shared" si="11"/>
         <v>17.45</v>
       </c>
-      <c r="L32" s="42">
+      <c r="L32" s="28">
         <f t="shared" si="12"/>
         <v>16.7</v>
       </c>
-      <c r="M32" s="61">
+      <c r="M32" s="34">
         <f t="shared" si="13"/>
         <v>15.95</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="46">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B33" s="33">
         <v>25</v>
       </c>
-      <c r="C33" s="41">
+      <c r="C33" s="28">
         <v>23.3</v>
       </c>
-      <c r="D33" s="41">
+      <c r="D33" s="28">
         <v>19.3</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="28">
         <f t="shared" si="5"/>
         <v>0.17167381974248927</v>
       </c>
-      <c r="F33" s="41">
+      <c r="F33" s="28">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="G33" s="46">
+      <c r="G33" s="33">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="H33" s="55">
+      <c r="H33" s="44">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="I33" s="61">
+      <c r="I33" s="34">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="J33" s="42">
+      <c r="J33" s="28">
         <f t="shared" si="10"/>
         <v>23.3</v>
       </c>
-      <c r="K33" s="42">
+      <c r="K33" s="28">
         <f t="shared" si="11"/>
         <v>22.3</v>
       </c>
-      <c r="L33" s="42">
+      <c r="L33" s="28">
         <f t="shared" si="12"/>
         <v>21.3</v>
       </c>
-      <c r="M33" s="61">
+      <c r="M33" s="34">
         <f t="shared" si="13"/>
         <v>20.3</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="46">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B34" s="33">
         <v>30</v>
       </c>
-      <c r="C34" s="45">
+      <c r="C34" s="36">
         <v>28.1</v>
       </c>
-      <c r="D34" s="45">
+      <c r="D34" s="36">
         <v>23.2</v>
       </c>
-      <c r="E34" s="45">
+      <c r="E34" s="36">
         <f t="shared" si="5"/>
         <v>0.17437722419928833</v>
       </c>
-      <c r="F34" s="41">
+      <c r="F34" s="28">
         <f t="shared" si="9"/>
         <v>4.9000000000000021</v>
       </c>
-      <c r="G34" s="46">
+      <c r="G34" s="33">
         <f t="shared" si="6"/>
         <v>1.2250000000000005</v>
       </c>
-      <c r="H34" s="55">
+      <c r="H34" s="44">
         <f t="shared" si="7"/>
         <v>2.4500000000000011</v>
       </c>
-      <c r="I34" s="61">
+      <c r="I34" s="34">
         <f t="shared" si="8"/>
         <v>3.6750000000000016</v>
       </c>
-      <c r="J34" s="42">
+      <c r="J34" s="28">
         <f t="shared" si="10"/>
         <v>28.1</v>
       </c>
-      <c r="K34" s="42">
+      <c r="K34" s="28">
         <f t="shared" si="11"/>
         <v>26.875</v>
       </c>
-      <c r="L34" s="42">
+      <c r="L34" s="28">
         <f t="shared" si="12"/>
         <v>25.65</v>
       </c>
-      <c r="M34" s="61">
+      <c r="M34" s="34">
         <f t="shared" si="13"/>
         <v>24.425000000000001</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="46">
+    <row r="35" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="33">
         <v>40</v>
       </c>
-      <c r="C35" s="42">
+      <c r="C35" s="28">
         <v>38.200000000000003</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="28">
         <v>31.4</v>
       </c>
-      <c r="E35" s="42">
+      <c r="E35" s="28">
         <f t="shared" si="5"/>
         <v>0.17801047120418859</v>
       </c>
-      <c r="F35" s="41">
+      <c r="F35" s="28">
         <f t="shared" si="9"/>
         <v>6.8000000000000043</v>
       </c>
-      <c r="G35" s="46">
+      <c r="G35" s="33">
         <f t="shared" si="6"/>
         <v>1.7000000000000011</v>
       </c>
-      <c r="H35" s="55">
+      <c r="H35" s="44">
         <f t="shared" si="7"/>
         <v>3.4000000000000021</v>
       </c>
-      <c r="I35" s="61">
+      <c r="I35" s="34">
         <f t="shared" si="8"/>
         <v>5.1000000000000032</v>
       </c>
-      <c r="J35" s="42">
+      <c r="J35" s="28">
         <f t="shared" si="10"/>
         <v>38.200000000000003</v>
       </c>
-      <c r="K35" s="42">
+      <c r="K35" s="28">
         <f t="shared" si="11"/>
         <v>36.5</v>
       </c>
-      <c r="L35" s="42">
+      <c r="L35" s="28">
         <f t="shared" si="12"/>
         <v>34.799999999999997</v>
       </c>
-      <c r="M35" s="61">
+      <c r="M35" s="34">
         <f t="shared" si="13"/>
         <v>33.1</v>
       </c>
     </row>
-    <row r="36" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="51">
+    <row r="36" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="40">
         <v>44.5</v>
       </c>
-      <c r="C36" s="52">
+      <c r="C36" s="41">
         <v>42.6</v>
       </c>
-      <c r="D36" s="52">
+      <c r="D36" s="41">
         <v>35.1</v>
       </c>
-      <c r="E36" s="52">
+      <c r="E36" s="41">
         <f t="shared" si="5"/>
         <v>0.176056338028169</v>
       </c>
-      <c r="F36" s="52">
+      <c r="F36" s="41">
         <f t="shared" si="9"/>
         <v>7.5</v>
       </c>
-      <c r="G36" s="51">
+      <c r="G36" s="40">
         <f t="shared" si="6"/>
         <v>1.875</v>
       </c>
-      <c r="H36" s="62">
+      <c r="H36" s="48">
         <f t="shared" si="7"/>
         <v>3.75</v>
       </c>
-      <c r="I36" s="53">
+      <c r="I36" s="42">
         <f t="shared" si="8"/>
         <v>5.625</v>
       </c>
-      <c r="J36" s="52">
+      <c r="J36" s="41">
         <f t="shared" si="10"/>
         <v>42.6</v>
       </c>
-      <c r="K36" s="52">
+      <c r="K36" s="41">
         <f t="shared" si="11"/>
         <v>40.725000000000001</v>
       </c>
-      <c r="L36" s="52">
+      <c r="L36" s="41">
         <f t="shared" si="12"/>
         <v>38.85</v>
       </c>
-      <c r="M36" s="53">
+      <c r="M36" s="42">
         <f t="shared" si="13"/>
         <v>36.975000000000001</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G38" s="34" t="s">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G38" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="H38" s="34" t="s">
+      <c r="H38" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="I38" s="34" t="s">
+      <c r="I38" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J38" s="34" t="s">
+      <c r="J38" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="K38" s="34" t="s">
+      <c r="K38" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="L38" s="34" t="s">
+      <c r="L38" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="34" t="s">
+    <row r="39" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F39" s="34" t="s">
+      <c r="F39" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="G39" s="34">
+      <c r="G39" s="28">
         <v>40.6</v>
       </c>
     </row>
-    <row r="40" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="56" t="s">
+    <row r="40" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="57" t="s">
+      <c r="C40" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="57" t="s">
+      <c r="D40" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="E40" s="57" t="s">
+      <c r="E40" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="57" t="s">
+      <c r="F40" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="56" t="s">
+      <c r="G40" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="H40" s="57" t="s">
+      <c r="H40" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="I40" s="57" t="s">
+      <c r="I40" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="J40" s="58" t="s">
+      <c r="J40" s="47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="46">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B41" s="33">
         <v>10</v>
       </c>
-      <c r="C41" s="41">
+      <c r="C41" s="28">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D41" s="41">
+      <c r="D41" s="28">
         <v>7</v>
       </c>
-      <c r="E41" s="41">
+      <c r="E41" s="28">
         <f t="shared" ref="E41:E48" si="14">(C41-D41)/C41</f>
         <v>0.15662650602409645</v>
       </c>
-      <c r="F41" s="41">
+      <c r="F41" s="28">
         <f>C41-D41</f>
         <v>1.3000000000000007</v>
       </c>
-      <c r="G41" s="46">
+      <c r="G41" s="33">
         <f>$G$39</f>
         <v>40.6</v>
       </c>
-      <c r="H41" s="42">
+      <c r="H41" s="28">
         <f>$G$39-G30</f>
         <v>40.274999999999999</v>
       </c>
-      <c r="I41" s="42">
+      <c r="I41" s="28">
         <f>$G$39-H30</f>
         <v>39.950000000000003</v>
       </c>
-      <c r="J41" s="61">
+      <c r="J41" s="34">
         <f>$G$39-I30</f>
         <v>39.625</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="46">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B42" s="33">
         <v>15</v>
       </c>
-      <c r="C42" s="41">
+      <c r="C42" s="28">
         <v>13.2</v>
       </c>
-      <c r="D42" s="41">
+      <c r="D42" s="28">
         <v>11.1</v>
       </c>
-      <c r="E42" s="41">
+      <c r="E42" s="28">
         <f t="shared" si="14"/>
         <v>0.15909090909090906</v>
       </c>
-      <c r="F42" s="41">
+      <c r="F42" s="28">
         <f t="shared" ref="F42:F48" si="15">C42-D42</f>
         <v>2.0999999999999996</v>
       </c>
-      <c r="G42" s="40">
+      <c r="G42" s="33">
         <v>45.3</v>
       </c>
-      <c r="H42" s="42">
+      <c r="H42" s="28">
         <f>$G$42-G31</f>
         <v>44.774999999999999</v>
       </c>
-      <c r="I42" s="42">
+      <c r="I42" s="28">
         <f t="shared" ref="I42:J42" si="16">$G$42-H31</f>
         <v>44.25</v>
       </c>
-      <c r="J42" s="61">
+      <c r="J42" s="34">
         <f t="shared" si="16"/>
         <v>43.724999999999994</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="46">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B43" s="33">
         <v>20</v>
       </c>
-      <c r="C43" s="41">
+      <c r="C43" s="28">
         <v>18.2</v>
       </c>
-      <c r="D43" s="41">
+      <c r="D43" s="28">
         <v>15.2</v>
       </c>
-      <c r="E43" s="41">
+      <c r="E43" s="28">
         <f t="shared" si="14"/>
         <v>0.16483516483516483</v>
       </c>
-      <c r="F43" s="41">
+      <c r="F43" s="28">
         <f t="shared" si="15"/>
         <v>3</v>
       </c>
-      <c r="G43" s="40">
+      <c r="G43" s="33">
         <v>50.5</v>
       </c>
-      <c r="H43" s="42">
+      <c r="H43" s="28">
         <f>G43-G32</f>
         <v>49.75</v>
       </c>
-      <c r="I43" s="42">
+      <c r="I43" s="28">
         <f>G43-H32</f>
         <v>49</v>
       </c>
-      <c r="J43" s="61">
+      <c r="J43" s="34">
         <f>G43-I32</f>
         <v>48.25</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="46">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B44" s="33">
         <v>25</v>
       </c>
-      <c r="C44" s="41">
+      <c r="C44" s="28">
         <v>23.3</v>
       </c>
-      <c r="D44" s="41">
+      <c r="D44" s="28">
         <v>19.3</v>
       </c>
-      <c r="E44" s="41">
+      <c r="E44" s="28">
         <f t="shared" si="14"/>
         <v>0.17167381974248927</v>
       </c>
-      <c r="F44" s="41">
+      <c r="F44" s="28">
         <f t="shared" si="15"/>
         <v>4</v>
       </c>
-      <c r="G44" s="40">
+      <c r="G44" s="33">
         <v>55.6</v>
       </c>
-      <c r="H44" s="42">
+      <c r="H44" s="28">
         <f>$G$44-G33</f>
         <v>54.6</v>
       </c>
-      <c r="I44" s="42">
+      <c r="I44" s="28">
         <f t="shared" ref="I44:J44" si="17">$G$44-H33</f>
         <v>53.6</v>
       </c>
-      <c r="J44" s="61">
+      <c r="J44" s="34">
         <f t="shared" si="17"/>
         <v>52.6</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="46">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B45" s="33">
         <v>30</v>
       </c>
-      <c r="C45" s="45">
+      <c r="C45" s="36">
         <v>28.1</v>
       </c>
-      <c r="D45" s="45">
+      <c r="D45" s="36">
         <v>23.2</v>
       </c>
-      <c r="E45" s="45">
+      <c r="E45" s="36">
         <f t="shared" si="14"/>
         <v>0.17437722419928833</v>
       </c>
-      <c r="F45" s="41">
+      <c r="F45" s="28">
         <f t="shared" si="15"/>
         <v>4.9000000000000021</v>
       </c>
-      <c r="G45" s="44">
+      <c r="G45" s="35">
         <v>60.5</v>
       </c>
-      <c r="H45" s="42">
+      <c r="H45" s="28">
         <f>$G$45-G34</f>
         <v>59.274999999999999</v>
       </c>
-      <c r="I45" s="42">
+      <c r="I45" s="28">
         <f>$G$45-H34</f>
         <v>58.05</v>
       </c>
-      <c r="J45" s="61">
+      <c r="J45" s="34">
         <f>$G$45-I34</f>
         <v>56.824999999999996</v>
       </c>
     </row>
-    <row r="46" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="47">
+    <row r="46" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="37">
         <v>40</v>
       </c>
-      <c r="C46" s="48">
+      <c r="C46" s="38">
         <v>38.200000000000003</v>
       </c>
-      <c r="D46" s="48">
+      <c r="D46" s="38">
         <v>31.4</v>
       </c>
-      <c r="E46" s="48">
+      <c r="E46" s="38">
         <f t="shared" si="14"/>
         <v>0.17801047120418859</v>
       </c>
-      <c r="F46" s="49">
+      <c r="F46" s="38">
         <f t="shared" si="15"/>
         <v>6.8000000000000043</v>
       </c>
-      <c r="G46" s="63">
+      <c r="G46" s="37">
         <v>70.7</v>
       </c>
-      <c r="H46" s="48">
+      <c r="H46" s="38">
         <f>$G$46-G35</f>
         <v>69</v>
       </c>
-      <c r="I46" s="48">
+      <c r="I46" s="38">
         <f t="shared" ref="I46:J46" si="18">$G$46-H35</f>
         <v>67.3</v>
       </c>
-      <c r="J46" s="64">
+      <c r="J46" s="39">
         <f t="shared" si="18"/>
         <v>65.599999999999994</v>
       </c>
     </row>
-    <row r="47" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="51">
+    <row r="47" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="40">
         <v>44.5</v>
       </c>
-      <c r="C47" s="52">
+      <c r="C47" s="41">
         <v>42.6</v>
       </c>
-      <c r="D47" s="52">
+      <c r="D47" s="41">
         <v>35.1</v>
       </c>
-      <c r="E47" s="52">
+      <c r="E47" s="41">
         <f t="shared" si="14"/>
         <v>0.176056338028169</v>
       </c>
-      <c r="F47" s="52">
+      <c r="F47" s="41">
         <f t="shared" si="15"/>
         <v>7.5</v>
       </c>
-      <c r="G47" s="51">
+      <c r="G47" s="40">
         <v>10000</v>
       </c>
-      <c r="H47" s="52">
+      <c r="H47" s="41">
         <f>$G$47-G26*F47</f>
         <v>9998.125</v>
       </c>
-      <c r="I47" s="52">
+      <c r="I47" s="41">
         <f>$G$47-G27*F47</f>
         <v>9996.25</v>
       </c>
-      <c r="J47" s="52">
+      <c r="J47" s="41">
         <f>$G$47-G28*F47</f>
         <v>9994.375</v>
       </c>
     </row>
-    <row r="48" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="65"/>
-      <c r="C48" s="66">
+    <row r="48" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="49"/>
+      <c r="C48" s="50">
         <v>52.1</v>
       </c>
-      <c r="D48" s="66">
+      <c r="D48" s="50">
         <v>43.7</v>
       </c>
-      <c r="E48" s="66">
+      <c r="E48" s="50">
         <f t="shared" si="14"/>
         <v>0.16122840690978885</v>
       </c>
-      <c r="F48" s="66">
+      <c r="F48" s="50">
         <f t="shared" si="15"/>
         <v>8.3999999999999986</v>
       </c>
-      <c r="G48" s="65">
+      <c r="G48" s="49">
         <v>84.5</v>
       </c>
-      <c r="H48" s="66">
+      <c r="H48" s="50">
         <f>$G$48-G26*F48</f>
         <v>82.4</v>
       </c>
-      <c r="I48" s="66">
+      <c r="I48" s="50">
         <f>$G$48-G27*F48</f>
         <v>80.3</v>
       </c>
-      <c r="J48" s="66">
+      <c r="J48" s="50">
         <f>$G$48-G28*F48</f>
         <v>78.2</v>
       </c>
@@ -4924,952 +4835,932 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323A83DE-7D7D-42B4-B230-E7B33C3EE77B}">
   <dimension ref="B1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="34"/>
-    <col min="2" max="2" width="16.85546875" style="34" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="47.7109375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="34" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="34"/>
+    <col min="1" max="1" width="9.109375" style="28"/>
+    <col min="2" max="2" width="16.88671875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="28" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="28" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="29">
         <v>10</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="30">
         <v>8.5</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="30">
         <v>6.7</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="30">
         <f t="shared" ref="E2:E7" si="0">(C2-D2)/C2</f>
         <v>0.21176470588235291</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="30">
         <f>C2-D2</f>
         <v>1.7999999999999998</v>
       </c>
-      <c r="G2" s="37">
+      <c r="G2" s="30">
         <f>B2-C2</f>
         <v>1.5</v>
       </c>
-      <c r="H2" s="38">
+      <c r="H2" s="31">
         <v>628</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="40">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="33">
         <v>15</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="28">
         <v>13.3</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="28">
         <v>10.3</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="28">
         <f t="shared" si="0"/>
         <v>0.22556390977443608</v>
       </c>
-      <c r="F3" s="41">
+      <c r="F3" s="28">
         <f t="shared" ref="F3:F7" si="1">C3-D3</f>
         <v>3</v>
       </c>
-      <c r="G3" s="42">
+      <c r="G3" s="28">
         <f t="shared" ref="G3:G7" si="2">B3-C3</f>
         <v>1.6999999999999993</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="51">
         <v>629</v>
       </c>
-      <c r="I3" s="43" t="s">
+      <c r="I3" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="40">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="33">
         <v>20</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="28">
         <v>18.3</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="28">
         <v>14.1</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="28">
         <f t="shared" si="0"/>
         <v>0.22950819672131154</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4" s="28">
         <f t="shared" si="1"/>
         <v>4.2000000000000011</v>
       </c>
-      <c r="G4" s="42">
+      <c r="G4" s="28">
         <f t="shared" si="2"/>
         <v>1.6999999999999993</v>
       </c>
-      <c r="H4" s="67">
+      <c r="H4" s="51">
         <v>630</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="40">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="33">
         <v>25</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="28">
         <v>23.3</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="28">
         <v>17.899999999999999</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="28">
         <f t="shared" si="0"/>
         <v>0.23175965665236059</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5" s="28">
         <f t="shared" si="1"/>
         <v>5.4000000000000021</v>
       </c>
-      <c r="G5" s="42">
+      <c r="G5" s="28">
         <f t="shared" si="2"/>
         <v>1.6999999999999993</v>
       </c>
-      <c r="H5" s="67">
+      <c r="H5" s="51">
         <v>631</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="44">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="35">
         <v>30</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="36">
         <v>28.2</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="36">
         <v>21.6</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="28">
         <f t="shared" si="0"/>
         <v>0.23404255319148928</v>
       </c>
-      <c r="F6" s="41">
+      <c r="F6" s="28">
         <f t="shared" si="1"/>
         <v>6.5999999999999979</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="28">
         <f t="shared" si="2"/>
         <v>1.8000000000000007</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="51">
         <v>632</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="47">
+    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="37">
         <v>40</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="38">
         <v>38.4</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="38">
         <v>29.5</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="38">
         <f t="shared" si="0"/>
         <v>0.23177083333333331</v>
       </c>
-      <c r="F7" s="49">
+      <c r="F7" s="38">
         <f t="shared" si="1"/>
         <v>8.8999999999999986</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="38">
         <f t="shared" si="2"/>
         <v>1.6000000000000014</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="52">
         <v>633</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="34" t="s">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="34" t="s">
+    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="29">
         <v>10</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36" t="e">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30" t="e">
         <f t="shared" ref="E16:E21" si="3">(C16-D16)/C16</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37">
+      <c r="F16" s="30"/>
+      <c r="G16" s="30">
         <f>B16-C16</f>
         <v>10</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="31">
         <v>830</v>
       </c>
-      <c r="I16" s="39" t="s">
+      <c r="I16" s="32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="40">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="33">
         <v>15</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41" t="e">
+      <c r="E17" s="28" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="42">
+      <c r="G17" s="28">
         <f t="shared" ref="G17:G21" si="4">B17-C17</f>
         <v>15</v>
       </c>
-      <c r="H17" s="41">
+      <c r="H17" s="28">
         <v>830</v>
       </c>
-      <c r="I17" s="43"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="40">
+      <c r="I17" s="34"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="33">
         <v>20</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41" t="e">
+      <c r="E18" s="28" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="42">
+      <c r="G18" s="28">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="43"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="40">
+      <c r="I18" s="34"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="33">
         <v>25</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41" t="e">
+      <c r="E19" s="28" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F19" s="41"/>
-      <c r="G19" s="42">
+      <c r="G19" s="28">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="H19" s="41"/>
-      <c r="I19" s="43"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="44">
+      <c r="I19" s="34"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="35">
         <v>30</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45" t="e">
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F20" s="45"/>
-      <c r="G20" s="42">
+      <c r="F20" s="36"/>
+      <c r="G20" s="28">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="H20" s="41"/>
-      <c r="I20" s="43"/>
-    </row>
-    <row r="21" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="47">
+      <c r="I20" s="34"/>
+    </row>
+    <row r="21" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="37">
         <v>40</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48" t="e">
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48">
+      <c r="F21" s="38"/>
+      <c r="G21" s="38">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="H21" s="48"/>
-      <c r="I21" s="50"/>
-    </row>
-    <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G23" s="34" t="s">
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
+    </row>
+    <row r="23" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G24" s="54">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G24" s="43">
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G25" s="55">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G25" s="44">
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="34" t="s">
+    <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G26" s="55">
+      <c r="G26" s="44">
         <v>0.75</v>
       </c>
-      <c r="J26" s="34" t="s">
+      <c r="J26" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="56" t="s">
+    <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="57" t="s">
+      <c r="D27" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="57" t="s">
+      <c r="E27" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="57" t="s">
+      <c r="F27" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="56" t="s">
+      <c r="G27" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="57" t="s">
+      <c r="H27" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="I27" s="58" t="s">
+      <c r="I27" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="57" t="s">
+      <c r="J27" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="K27" s="57" t="s">
+      <c r="K27" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="L27" s="57" t="s">
+      <c r="L27" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="M27" s="58" t="s">
+      <c r="M27" s="47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="46">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="33">
         <v>10</v>
       </c>
-      <c r="C28" s="36">
+      <c r="C28" s="30">
         <v>8.5</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="30">
         <v>6.7</v>
       </c>
-      <c r="E28" s="41">
+      <c r="E28" s="28">
         <f t="shared" ref="E28:E33" si="5">(C28-D28)/C28</f>
         <v>0.21176470588235291</v>
       </c>
-      <c r="F28" s="41">
+      <c r="F28" s="28">
         <f>C28-D28</f>
         <v>1.7999999999999998</v>
       </c>
-      <c r="G28" s="46">
+      <c r="G28" s="33">
         <f t="shared" ref="G28:G33" si="6">$G$24*F28</f>
         <v>0.44999999999999996</v>
       </c>
-      <c r="H28" s="42">
+      <c r="H28" s="28">
         <f t="shared" ref="H28:H33" si="7">$G$25*F28</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="I28" s="61">
+      <c r="I28" s="34">
         <f t="shared" ref="I28:I33" si="8">$G$26*F28</f>
         <v>1.3499999999999999</v>
       </c>
-      <c r="J28" s="42">
+      <c r="J28" s="28">
         <f>C28</f>
         <v>8.5</v>
       </c>
-      <c r="K28" s="42">
+      <c r="K28" s="28">
         <f>C28-G28</f>
         <v>8.0500000000000007</v>
       </c>
-      <c r="L28" s="42">
+      <c r="L28" s="28">
         <f>C28-H28</f>
         <v>7.6</v>
       </c>
-      <c r="M28" s="61">
+      <c r="M28" s="34">
         <f>C28-I28</f>
         <v>7.15</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="46">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B29" s="33">
         <v>15</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="28">
         <v>13.3</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D29" s="28">
         <v>10.3</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="28">
         <f t="shared" si="5"/>
         <v>0.22556390977443608</v>
       </c>
-      <c r="F29" s="41">
+      <c r="F29" s="28">
         <f t="shared" ref="F29:F33" si="9">C29-D29</f>
         <v>3</v>
       </c>
-      <c r="G29" s="46">
+      <c r="G29" s="33">
         <f t="shared" si="6"/>
         <v>0.75</v>
       </c>
-      <c r="H29" s="42">
+      <c r="H29" s="28">
         <f t="shared" si="7"/>
         <v>1.5</v>
       </c>
-      <c r="I29" s="61">
+      <c r="I29" s="34">
         <f t="shared" si="8"/>
         <v>2.25</v>
       </c>
-      <c r="J29" s="42">
+      <c r="J29" s="28">
         <f t="shared" ref="J29:J33" si="10">C29</f>
         <v>13.3</v>
       </c>
-      <c r="K29" s="42">
+      <c r="K29" s="28">
         <f t="shared" ref="K29:K33" si="11">C29-G29</f>
         <v>12.55</v>
       </c>
-      <c r="L29" s="42">
+      <c r="L29" s="28">
         <f t="shared" ref="L29:L33" si="12">C29-H29</f>
         <v>11.8</v>
       </c>
-      <c r="M29" s="61">
+      <c r="M29" s="34">
         <f t="shared" ref="M29:M33" si="13">C29-I29</f>
         <v>11.05</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="46">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="33">
         <v>20</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="28">
         <v>18.3</v>
       </c>
-      <c r="D30" s="41">
+      <c r="D30" s="28">
         <v>14.1</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="28">
         <f t="shared" si="5"/>
         <v>0.22950819672131154</v>
       </c>
-      <c r="F30" s="41">
+      <c r="F30" s="28">
         <f t="shared" si="9"/>
         <v>4.2000000000000011</v>
       </c>
-      <c r="G30" s="46">
+      <c r="G30" s="33">
         <f t="shared" si="6"/>
         <v>1.0500000000000003</v>
       </c>
-      <c r="H30" s="42">
+      <c r="H30" s="28">
         <f t="shared" si="7"/>
         <v>2.1000000000000005</v>
       </c>
-      <c r="I30" s="61">
+      <c r="I30" s="34">
         <f t="shared" si="8"/>
         <v>3.1500000000000008</v>
       </c>
-      <c r="J30" s="42">
+      <c r="J30" s="28">
         <f t="shared" si="10"/>
         <v>18.3</v>
       </c>
-      <c r="K30" s="42">
+      <c r="K30" s="28">
         <f t="shared" si="11"/>
         <v>17.25</v>
       </c>
-      <c r="L30" s="42">
+      <c r="L30" s="28">
         <f t="shared" si="12"/>
         <v>16.2</v>
       </c>
-      <c r="M30" s="61">
+      <c r="M30" s="34">
         <f t="shared" si="13"/>
         <v>15.15</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="46">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="33">
         <v>25</v>
       </c>
-      <c r="C31" s="41">
+      <c r="C31" s="28">
         <v>23.3</v>
       </c>
-      <c r="D31" s="41">
+      <c r="D31" s="28">
         <v>17.899999999999999</v>
       </c>
-      <c r="E31" s="41">
+      <c r="E31" s="28">
         <f t="shared" si="5"/>
         <v>0.23175965665236059</v>
       </c>
-      <c r="F31" s="41">
+      <c r="F31" s="28">
         <f t="shared" si="9"/>
         <v>5.4000000000000021</v>
       </c>
-      <c r="G31" s="46">
+      <c r="G31" s="33">
         <f t="shared" si="6"/>
         <v>1.3500000000000005</v>
       </c>
-      <c r="H31" s="42">
+      <c r="H31" s="28">
         <f t="shared" si="7"/>
         <v>2.7000000000000011</v>
       </c>
-      <c r="I31" s="61">
+      <c r="I31" s="34">
         <f t="shared" si="8"/>
         <v>4.0500000000000016</v>
       </c>
-      <c r="J31" s="42">
+      <c r="J31" s="28">
         <f t="shared" si="10"/>
         <v>23.3</v>
       </c>
-      <c r="K31" s="42">
+      <c r="K31" s="28">
         <f t="shared" si="11"/>
         <v>21.95</v>
       </c>
-      <c r="L31" s="42">
+      <c r="L31" s="28">
         <f t="shared" si="12"/>
         <v>20.6</v>
       </c>
-      <c r="M31" s="61">
+      <c r="M31" s="34">
         <f t="shared" si="13"/>
         <v>19.25</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="46">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="33">
         <v>30</v>
       </c>
-      <c r="C32" s="45">
+      <c r="C32" s="36">
         <v>28.2</v>
       </c>
-      <c r="D32" s="45">
+      <c r="D32" s="36">
         <v>21.6</v>
       </c>
-      <c r="E32" s="45">
+      <c r="E32" s="36">
         <f t="shared" si="5"/>
         <v>0.23404255319148928</v>
       </c>
-      <c r="F32" s="41">
+      <c r="F32" s="28">
         <f t="shared" si="9"/>
         <v>6.5999999999999979</v>
       </c>
-      <c r="G32" s="46">
+      <c r="G32" s="33">
         <f t="shared" si="6"/>
         <v>1.6499999999999995</v>
       </c>
-      <c r="H32" s="42">
+      <c r="H32" s="28">
         <f t="shared" si="7"/>
         <v>3.2999999999999989</v>
       </c>
-      <c r="I32" s="61">
+      <c r="I32" s="34">
         <f t="shared" si="8"/>
         <v>4.9499999999999984</v>
       </c>
-      <c r="J32" s="42">
+      <c r="J32" s="28">
         <f t="shared" si="10"/>
         <v>28.2</v>
       </c>
-      <c r="K32" s="42">
+      <c r="K32" s="28">
         <f t="shared" si="11"/>
         <v>26.55</v>
       </c>
-      <c r="L32" s="42">
+      <c r="L32" s="28">
         <f t="shared" si="12"/>
         <v>24.9</v>
       </c>
-      <c r="M32" s="61">
+      <c r="M32" s="34">
         <f t="shared" si="13"/>
         <v>23.25</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="47">
+    <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="37">
         <v>40</v>
       </c>
-      <c r="C33" s="48">
+      <c r="C33" s="38">
         <v>38.4</v>
       </c>
-      <c r="D33" s="48">
+      <c r="D33" s="38">
         <v>29.5</v>
       </c>
-      <c r="E33" s="48">
+      <c r="E33" s="38">
         <f t="shared" si="5"/>
         <v>0.23177083333333331</v>
       </c>
-      <c r="F33" s="49">
+      <c r="F33" s="38">
         <f t="shared" si="9"/>
         <v>8.8999999999999986</v>
       </c>
-      <c r="G33" s="47">
+      <c r="G33" s="37">
         <f t="shared" si="6"/>
         <v>2.2249999999999996</v>
       </c>
-      <c r="H33" s="48">
+      <c r="H33" s="38">
         <f t="shared" si="7"/>
         <v>4.4499999999999993</v>
       </c>
-      <c r="I33" s="64">
+      <c r="I33" s="39">
         <f t="shared" si="8"/>
         <v>6.6749999999999989</v>
       </c>
-      <c r="J33" s="48">
+      <c r="J33" s="38">
         <f t="shared" si="10"/>
         <v>38.4</v>
       </c>
-      <c r="K33" s="48">
+      <c r="K33" s="38">
         <f t="shared" si="11"/>
         <v>36.174999999999997</v>
       </c>
-      <c r="L33" s="48">
+      <c r="L33" s="38">
         <f t="shared" si="12"/>
         <v>33.950000000000003</v>
       </c>
-      <c r="M33" s="64">
+      <c r="M33" s="39">
         <f t="shared" si="13"/>
         <v>31.725000000000001</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G35" s="34" t="s">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G35" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="H35" s="34" t="s">
+      <c r="H35" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="I35" s="34" t="s">
+      <c r="I35" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J35" s="34" t="s">
+      <c r="J35" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="K35" s="34" t="s">
+      <c r="K35" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="L35" s="34" t="s">
+      <c r="L35" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="34" t="s">
+    <row r="36" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="F36" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="G36" s="34">
+      <c r="G36" s="28">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="56" t="s">
+    <row r="37" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="57" t="s">
+      <c r="C37" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D37" s="57" t="s">
+      <c r="D37" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="57" t="s">
+      <c r="E37" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="57" t="s">
+      <c r="F37" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="56" t="s">
+      <c r="G37" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="H37" s="57" t="s">
+      <c r="H37" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="57" t="s">
+      <c r="I37" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="J37" s="58" t="s">
+      <c r="J37" s="47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="46">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B38" s="33">
         <v>10</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41" t="e">
+      <c r="E38" s="28" t="e">
         <f t="shared" ref="E38:E43" si="14">(C38-D38)/C38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F38" s="41">
+      <c r="F38" s="28">
         <f>C38-D38</f>
         <v>0</v>
       </c>
-      <c r="G38" s="46">
+      <c r="G38" s="33">
         <v>40</v>
       </c>
-      <c r="H38" s="42">
+      <c r="H38" s="28">
         <f>$G$36-G28</f>
         <v>39.549999999999997</v>
       </c>
-      <c r="I38" s="42">
+      <c r="I38" s="28">
         <f>$G$36-H28</f>
         <v>39.1</v>
       </c>
-      <c r="J38" s="61">
+      <c r="J38" s="34">
         <f>$G$36-I28</f>
         <v>38.65</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="46">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B39" s="33">
         <v>15</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41" t="e">
+      <c r="E39" s="28" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F39" s="41">
+      <c r="F39" s="28">
         <f t="shared" ref="F39:F43" si="15">C39-D39</f>
         <v>0</v>
       </c>
-      <c r="G39" s="40"/>
-      <c r="H39" s="42">
+      <c r="G39" s="33"/>
+      <c r="H39" s="28">
         <f>$G$39-G29</f>
         <v>-0.75</v>
       </c>
-      <c r="I39" s="42">
+      <c r="I39" s="28">
         <f t="shared" ref="I39:J39" si="16">$G$39-H29</f>
         <v>-1.5</v>
       </c>
-      <c r="J39" s="61">
+      <c r="J39" s="34">
         <f t="shared" si="16"/>
         <v>-2.25</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="46">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B40" s="33">
         <v>20</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41" t="e">
+      <c r="E40" s="28" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F40" s="41">
+      <c r="F40" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G40" s="40"/>
-      <c r="H40" s="42">
+      <c r="G40" s="33"/>
+      <c r="H40" s="28">
         <f>G40-G30</f>
         <v>-1.0500000000000003</v>
       </c>
-      <c r="I40" s="42">
+      <c r="I40" s="28">
         <f>G40-H30</f>
         <v>-2.1000000000000005</v>
       </c>
-      <c r="J40" s="61">
+      <c r="J40" s="34">
         <f>G40-I30</f>
         <v>-3.1500000000000008</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="46">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B41" s="33">
         <v>25</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41" t="e">
+      <c r="E41" s="28" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F41" s="41">
+      <c r="F41" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G41" s="40"/>
-      <c r="H41" s="42">
+      <c r="G41" s="33"/>
+      <c r="H41" s="28">
         <f>$G$41-G31</f>
         <v>-1.3500000000000005</v>
       </c>
-      <c r="I41" s="42">
+      <c r="I41" s="28">
         <f t="shared" ref="I41:J41" si="17">$G$41-H31</f>
         <v>-2.7000000000000011</v>
       </c>
-      <c r="J41" s="61">
+      <c r="J41" s="34">
         <f t="shared" si="17"/>
         <v>-4.0500000000000016</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="46">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B42" s="33">
         <v>30</v>
       </c>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45" t="e">
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F42" s="41">
+      <c r="F42" s="28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G42" s="44"/>
-      <c r="H42" s="42">
+      <c r="G42" s="35"/>
+      <c r="H42" s="28">
         <f>$G$42-G32</f>
         <v>-1.6499999999999995</v>
       </c>
-      <c r="I42" s="42">
+      <c r="I42" s="28">
         <f>$G$42-H32</f>
         <v>-3.2999999999999989</v>
       </c>
-      <c r="J42" s="61">
+      <c r="J42" s="34">
         <f>$G$42-I32</f>
         <v>-4.9499999999999984</v>
       </c>
     </row>
-    <row r="43" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="47">
+    <row r="43" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="37">
         <v>40</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48" t="e">
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F43" s="49">
+      <c r="F43" s="38">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G43" s="63"/>
-      <c r="H43" s="48">
+      <c r="G43" s="37"/>
+      <c r="H43" s="38">
         <f>$G$43-G33</f>
         <v>-2.2249999999999996</v>
       </c>
-      <c r="I43" s="48">
+      <c r="I43" s="38">
         <f t="shared" ref="I43:J43" si="18">$G$43-H33</f>
         <v>-4.4499999999999993</v>
       </c>
-      <c r="J43" s="64">
+      <c r="J43" s="39">
         <f t="shared" si="18"/>
         <v>-6.6749999999999989</v>
       </c>
@@ -5889,15 +5780,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5923,8 +5814,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="26">
         <v>12.4</v>
       </c>
       <c r="B2" s="2">
@@ -5933,10 +5824,10 @@
       <c r="C2" s="2">
         <v>7.4</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="3">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1">
@@ -5948,47 +5839,41 @@
       <c r="J2" s="2">
         <v>7.4</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="19">
         <v>9.8000000000000007</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>8.5</v>
       </c>
-      <c r="E3" s="5"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="26">
+      <c r="K3" s="20">
         <v>8.5</v>
       </c>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9">
+    </row>
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8">
         <v>7.8</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="27">
+      <c r="E4" s="9"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="21">
         <v>7.8</v>
       </c>
-      <c r="L4" s="23"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="26">
         <v>15</v>
       </c>
       <c r="B5" s="2">
@@ -5997,10 +5882,10 @@
       <c r="C5" s="2">
         <v>9.5</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="3">
         <v>12</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="1">
@@ -6012,47 +5897,43 @@
       <c r="J5" s="2">
         <v>9.5</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="19">
         <v>12</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="12">
+      <c r="D6" s="5">
         <v>11</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="9"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="26">
+      <c r="K6" s="20">
         <v>11</v>
       </c>
-      <c r="L6" s="23"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="13">
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8">
         <v>10</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="27">
+      <c r="E7" s="9"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="21">
         <v>10</v>
       </c>
-      <c r="L7" s="23"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="26">
         <v>25.3</v>
       </c>
       <c r="B8" s="2">
@@ -6061,10 +5942,10 @@
       <c r="C8" s="2">
         <v>17.3</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="3">
         <v>22.8</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="1">
@@ -6076,47 +5957,43 @@
       <c r="J8" s="2">
         <v>17.3</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="19">
         <v>22.8</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="L8" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="12">
+      <c r="D9" s="5">
         <v>21.9</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="9"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="26">
+      <c r="K9" s="20">
         <v>21.9</v>
       </c>
-      <c r="L9" s="23"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="13">
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8">
         <v>20.9</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="27">
+      <c r="E10" s="9"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="21">
         <v>20.9</v>
       </c>
-      <c r="L10" s="23"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="32">
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="26">
         <v>30</v>
       </c>
       <c r="B11" s="2">
@@ -6125,10 +6002,10 @@
       <c r="C11" s="2">
         <v>20.7</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="3">
         <v>27.5</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="1">
@@ -6140,63 +6017,55 @@
       <c r="J11" s="2">
         <v>20.7</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="19">
         <v>27.5</v>
       </c>
-      <c r="L11" s="23" t="s">
+      <c r="L11" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="12">
+      <c r="D12" s="5">
         <v>26.1</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="9"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="26">
+      <c r="K12" s="20">
         <v>26.1</v>
       </c>
-      <c r="L12" s="23"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="12">
+      <c r="D13" s="5">
         <v>25.2</v>
       </c>
-      <c r="E13" s="23"/>
+      <c r="E13" s="9"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="26">
+      <c r="K13" s="20">
         <v>25.2</v>
       </c>
-      <c r="L13" s="23"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="13">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8">
         <v>24.1</v>
       </c>
-      <c r="E14" s="23"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="27">
+      <c r="E14" s="9"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="21">
         <v>24.1</v>
       </c>
-      <c r="L14" s="23"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="32">
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="26">
         <v>42.7</v>
       </c>
       <c r="B15" s="2">
@@ -6205,10 +6074,10 @@
       <c r="C15" s="2">
         <v>29.6</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="3">
         <v>39.700000000000003</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="1">
@@ -6220,74 +6089,68 @@
       <c r="J15" s="2">
         <v>29.6</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="19">
         <v>39.700000000000003</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="12">
+      <c r="D16" s="5">
         <v>36.200000000000003</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="9"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="26">
+      <c r="K16" s="20">
         <v>36.200000000000003</v>
       </c>
-      <c r="L16" s="23"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="14">
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="10">
         <v>35.1</v>
       </c>
-      <c r="E17" s="23"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="29">
+      <c r="E17" s="9"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="23">
         <v>35.1</v>
       </c>
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18">
         <v>32.799999999999997</v>
       </c>
-      <c r="E18" s="23"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="30">
+      <c r="E18" s="9"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="24">
         <v>32.799999999999997</v>
       </c>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="5"/>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6302,13 +6165,13 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6325,20 +6188,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="26">
         <v>12.5</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="27">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="27">
         <v>7.6</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="19">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G2">
@@ -6346,46 +6209,43 @@
         <v>2.2000000000000011</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="26">
+      <c r="D3" s="20">
         <v>8.5</v>
       </c>
-      <c r="E3" s="5"/>
       <c r="G3">
         <f t="shared" ref="G3:G15" si="0">B3-C3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="27">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="21">
         <v>7.8</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="9"/>
       <c r="G4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="26">
         <v>14.8</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="27">
         <v>12</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="27">
         <v>9.1</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="19">
         <v>12</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="G5">
@@ -6393,46 +6253,44 @@
         <v>2.9000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="26">
+      <c r="D6" s="20">
         <v>11</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="9"/>
       <c r="G6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="27">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="21">
         <v>10</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="9"/>
       <c r="G7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="26">
         <v>25.2</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="27">
         <v>22.5</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="27">
         <v>17</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="19">
         <v>22.8</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G8">
@@ -6440,46 +6298,44 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="26">
+      <c r="D9" s="20">
         <v>21.9</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="9"/>
       <c r="G9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="27">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="21">
         <v>20.9</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="9"/>
       <c r="G10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="32">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="26">
         <v>30</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="27">
         <v>27.4</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="27">
         <v>20.7</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="19">
         <v>27.5</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G11">
@@ -6487,59 +6343,55 @@
         <v>6.6999999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="26">
+      <c r="D12" s="20">
         <v>26.1</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="9"/>
       <c r="G12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="26">
+      <c r="D13" s="20">
         <v>25.2</v>
       </c>
-      <c r="E13" s="23"/>
+      <c r="E13" s="9"/>
       <c r="G13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="27">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="21">
         <v>24.1</v>
       </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="9"/>
       <c r="G14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="32">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="26">
         <v>42.6</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="27">
         <v>39.799999999999997</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="27">
         <v>29.9</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="19">
         <v>39.700000000000003</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G15">
@@ -6547,32 +6399,30 @@
         <v>9.8999999999999986</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="26">
+      <c r="D16" s="20">
         <v>36.200000000000003</v>
       </c>
-      <c r="E16" s="23"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="29">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="23">
         <v>35.1</v>
       </c>
-      <c r="E17" s="23"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="30">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="24">
         <v>32.799999999999997</v>
       </c>
-      <c r="E18" s="23"/>
+      <c r="E18" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
attempting mat to csv conversion
</commit_message>
<xml_diff>
--- a/BPA_Static_Characterization_Test/DataCollection/BPAparameters_.xlsx
+++ b/BPA_Static_Characterization_Test/DataCollection/BPAparameters_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Muscle_Sensory\BPA_Static_Characterization_Test\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A6BB67-76D0-4128-9B37-099F9980B91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5530C2-E8EE-4116-81EC-ADBAFC082A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6BFF55C1-2CC5-46ED-9297-2ED97EF982C6}"/>
   </bookViews>
@@ -3704,8 +3704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6CD35F-74A9-469A-95AE-E3CD27253D58}">
   <dimension ref="B1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
+      <selection activeCell="M31" sqref="J31:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>